<commit_message>
update excel for consistency with r code
</commit_message>
<xml_diff>
--- a/states and actions.xlsx
+++ b/states and actions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domberg\Desktop\studies\2019 ARG2\simulations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anselm/github/arg2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64570435-D7E8-3D4C-A7A8-2C661EB357A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="41280" windowHeight="13512"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -17,28 +18,34 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$B$1:$L$90</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Domberg, Andreas</author>
   </authors>
   <commentList>
-    <comment ref="J4" authorId="0" shapeId="0">
+    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
@@ -47,17 +54,26 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-only really unnecessary if A turns out short
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">only really unnecessary if A turns out short
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="H36" authorId="0" shapeId="0">
+    <comment ref="H36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -87,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="35">
   <si>
     <t>rare</t>
   </si>
@@ -131,12 +147,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>full</t>
   </si>
   <si>
@@ -186,32 +196,31 @@
   </si>
   <si>
     <t>RR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ </t>
+  </si>
+  <si>
+    <t>__</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>long</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -225,6 +234,19 @@
       <color indexed="81"/>
       <name val="Segoe UI"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -313,6 +335,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -322,17 +350,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -358,156 +380,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -842,65 +714,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U90"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:T90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="181" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="13" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" customWidth="1"/>
-    <col min="2" max="7" width="5.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="7" width="5.83203125" style="1" customWidth="1"/>
     <col min="8" max="12" width="5.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="52.5546875" customWidth="1"/>
+    <col min="14" max="14" width="52.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="2:20">
+      <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="O1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:20">
       <c r="B2" s="2"/>
-      <c r="C2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="7"/>
+      <c r="C2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="9"/>
       <c r="G2" s="4"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="O2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -916,7 +788,9 @@
       <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
@@ -932,19 +806,22 @@
       <c r="L3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="M3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20">
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -958,10 +835,10 @@
         <v>x</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K4" s="2" t="str">
         <f>IF(OR(C4="full",E4="x"),"x","")</f>
@@ -971,105 +848,105 @@
         <f>IF(OR(D4="full",F4="x"),"x","")</f>
         <v>x</v>
       </c>
-      <c r="O4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="N4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20">
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I5" s="2" t="str">
         <f>IF(E5&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L5" s="2" t="str">
         <f>IF(OR(D5="full",F5="x"),"x","")</f>
         <v>x</v>
       </c>
-      <c r="O5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="N5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20">
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I6" s="2" t="str">
         <f>IF(E6&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L6" s="2" t="str">
         <f>IF(OR(D6="full",F6="x"),"x","")</f>
         <v>x</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:20">
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>19</v>
+        <v>30</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="J7" s="2" t="str">
         <f t="shared" ref="J7:J12" si="0">IF(F7&lt;&gt;"x","x","")</f>
@@ -1080,31 +957,31 @@
         <v>x</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1115,28 +992,28 @@
         <v>x</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20">
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I9" s="2" t="str">
         <f>IF(E9&lt;&gt;"x","x","")</f>
@@ -1147,31 +1024,31 @@
         <v>x</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20">
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I10" s="2" t="str">
         <f>IF(E10&lt;&gt;"x","x","")</f>
@@ -1182,31 +1059,31 @@
         <v>x</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20">
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I11" s="2" t="str">
         <f>IF(E11&lt;&gt;"x","x","")</f>
@@ -1217,36 +1094,36 @@
         <v>x</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:20">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I12" s="2" t="str">
         <f>IF(E12&lt;&gt;"x","x","")</f>
@@ -1257,21 +1134,21 @@
         <v>x</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20">
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>13</v>
@@ -1285,10 +1162,10 @@
         <v>x</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K13" s="2" t="str">
         <f t="shared" ref="K13:L15" si="1">IF(OR(C13="full",E13="x"),"x","")</f>
@@ -1299,32 +1176,32 @@
         <v>x</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:20">
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I14" s="2" t="str">
         <f>IF(E14&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K14" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1335,32 +1212,32 @@
         <v>x</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20">
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I15" s="2" t="str">
         <f>IF(E15&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K15" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1371,28 +1248,28 @@
         <v>x</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20">
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J16" s="2" t="str">
         <f t="shared" ref="J16:J21" si="2">IF(F16&lt;&gt;"x","x","")</f>
@@ -1403,31 +1280,31 @@
         <v>x</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
       <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J17" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1438,28 +1315,28 @@
         <v>x</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I18" s="2" t="str">
         <f>IF(E18&lt;&gt;"x","x","")</f>
@@ -1474,28 +1351,28 @@
         <v>x</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I19" s="2" t="str">
         <f>IF(E19&lt;&gt;"x","x","")</f>
@@ -1510,28 +1387,28 @@
         <v>x</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12">
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I20" s="2" t="str">
         <f>IF(E20&lt;&gt;"x","x","")</f>
@@ -1546,28 +1423,28 @@
         <v>x</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12">
       <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I21" s="2" t="str">
         <f>IF(E21&lt;&gt;"x","x","")</f>
@@ -1582,18 +1459,18 @@
         <v>x</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12">
       <c r="B22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>13</v>
@@ -1607,10 +1484,10 @@
         <v>x</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K22" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1621,98 +1498,98 @@
         <v>x</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12">
       <c r="B23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I23" s="2" t="str">
         <f>IF(E23&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L23" s="2" t="str">
         <f t="shared" si="4"/>
         <v>x</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12">
       <c r="B24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I24" s="2" t="str">
         <f>IF(E24&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="L24" s="2" t="str">
         <f t="shared" si="4"/>
         <v>x</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12">
       <c r="B25" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J25" s="2" t="str">
         <f t="shared" ref="J25:J30" si="5">IF(F25&lt;&gt;"x","x","")</f>
@@ -1727,28 +1604,28 @@
         <v>x</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12">
       <c r="B26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J26" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1763,25 +1640,25 @@
         <v>x</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12">
       <c r="B27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I27" s="2" t="str">
         <f>IF(E27&lt;&gt;"x","x","")</f>
@@ -1792,32 +1669,32 @@
         <v>x</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L27" s="2" t="str">
         <f t="shared" si="4"/>
         <v>x</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12">
       <c r="B28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I28" s="2" t="str">
         <f>IF(E28&lt;&gt;"x","x","")</f>
@@ -1828,32 +1705,32 @@
         <v>x</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L28" s="2" t="str">
         <f t="shared" si="4"/>
         <v>x</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12">
       <c r="B29" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I29" s="2" t="str">
         <f>IF(E29&lt;&gt;"x","x","")</f>
@@ -1864,32 +1741,32 @@
         <v>x</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L29" s="2" t="str">
         <f t="shared" si="4"/>
         <v>x</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12">
       <c r="B30" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I30" s="2" t="str">
         <f>IF(E30&lt;&gt;"x","x","")</f>
@@ -1900,22 +1777,22 @@
         <v>x</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L30" s="2" t="str">
         <f t="shared" si="4"/>
         <v>x</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12">
       <c r="B31" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>13</v>
@@ -1929,10 +1806,10 @@
         <v>x</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K31" s="2" t="str">
         <f>IF(OR(C31="full",E31="x"),"x","")</f>
@@ -1943,98 +1820,98 @@
         <v>x</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12">
       <c r="B32" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I32" s="2" t="str">
         <f>IF(E32&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L32" s="2" t="str">
         <f t="shared" si="4"/>
         <v>x</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12">
       <c r="B33" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I33" s="2" t="str">
         <f>IF(E33&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L33" s="2" t="str">
         <f t="shared" si="4"/>
         <v>x</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12">
       <c r="B34" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J34" s="2" t="str">
         <f t="shared" ref="J34:J39" si="6">IF(F34&lt;&gt;"x","x","")</f>
@@ -2045,31 +1922,31 @@
         <v>x</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12">
       <c r="B35" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J35" s="2" t="str">
         <f t="shared" si="6"/>
@@ -2080,28 +1957,28 @@
         <v>x</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12">
       <c r="B36" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I36" s="2" t="str">
         <f>IF(E36&lt;&gt;"x","x","")</f>
@@ -2112,31 +1989,31 @@
         <v>x</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12">
       <c r="B37" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I37" s="2" t="str">
         <f>IF(E37&lt;&gt;"x","x","")</f>
@@ -2147,31 +2024,31 @@
         <v>x</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12">
       <c r="B38" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I38" s="2" t="str">
         <f>IF(E38&lt;&gt;"x","x","")</f>
@@ -2182,31 +2059,31 @@
         <v>x</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12">
       <c r="B39" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I39" s="2" t="str">
         <f>IF(E39&lt;&gt;"x","x","")</f>
@@ -2217,21 +2094,21 @@
         <v>x</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12">
       <c r="B40" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>13</v>
@@ -2245,10 +2122,10 @@
         <v>x</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K40" s="2" t="str">
         <f t="shared" ref="K40:L42" si="7">IF(OR(C40="full",E40="x"),"x","")</f>
@@ -2259,32 +2136,32 @@
         <v>x</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12">
       <c r="B41" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I41" s="2" t="str">
         <f>IF(E41&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K41" s="2" t="str">
         <f t="shared" si="7"/>
@@ -2295,32 +2172,32 @@
         <v>x</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12">
       <c r="B42" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G42" s="2"/>
-      <c r="H42" s="9" t="s">
-        <v>27</v>
+      <c r="H42" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="I42" s="2" t="str">
         <f>IF(E42&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K42" s="2" t="str">
         <f t="shared" si="7"/>
@@ -2331,28 +2208,28 @@
         <v>x</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12">
       <c r="B43" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J43" s="2" t="str">
         <f t="shared" ref="J43:J48" si="8">IF(F43&lt;&gt;"x","x","")</f>
@@ -2363,31 +2240,31 @@
         <v>x</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12">
       <c r="B44" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J44" s="2" t="str">
         <f t="shared" si="8"/>
@@ -2398,28 +2275,28 @@
         <v>x</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12">
       <c r="B45" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I45" s="2" t="str">
         <f>IF(E45&lt;&gt;"x","x","")</f>
@@ -2434,28 +2311,28 @@
         <v>x</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12">
       <c r="B46" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I46" s="2" t="str">
         <f>IF(E46&lt;&gt;"x","x","")</f>
@@ -2470,28 +2347,28 @@
         <v>x</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12">
       <c r="B47" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I47" s="2" t="str">
         <f>IF(E47&lt;&gt;"x","x","")</f>
@@ -2506,28 +2383,28 @@
         <v>x</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12">
       <c r="B48" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I48" s="2" t="str">
         <f>IF(E48&lt;&gt;"x","x","")</f>
@@ -2542,18 +2419,18 @@
         <v>x</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12">
       <c r="B49" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>13</v>
@@ -2567,10 +2444,10 @@
         <v>x</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K49" s="2" t="str">
         <f t="shared" si="9"/>
@@ -2581,98 +2458,98 @@
         <v>x</v>
       </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:12">
       <c r="B50" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I50" s="2" t="str">
         <f>IF(E50&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L50" s="2" t="str">
         <f t="shared" si="10"/>
         <v>x</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:12">
       <c r="B51" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I51" s="2" t="str">
         <f>IF(E51&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K51" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="L51" s="2" t="str">
         <f t="shared" si="10"/>
         <v>x</v>
       </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:12">
       <c r="B52" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J52" s="2" t="str">
         <f t="shared" ref="J52:J57" si="11">IF(F52&lt;&gt;"x","x","")</f>
@@ -2687,28 +2564,28 @@
         <v>x</v>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:12">
       <c r="B53" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J53" s="2" t="str">
         <f t="shared" si="11"/>
@@ -2723,25 +2600,25 @@
         <v>x</v>
       </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:12">
       <c r="B54" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I54" s="2" t="str">
         <f>IF(E54&lt;&gt;"x","x","")</f>
@@ -2752,32 +2629,32 @@
         <v>x</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L54" s="2" t="str">
         <f t="shared" si="10"/>
         <v>x</v>
       </c>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:12">
       <c r="B55" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I55" s="2" t="str">
         <f>IF(E55&lt;&gt;"x","x","")</f>
@@ -2788,32 +2665,32 @@
         <v>x</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L55" s="2" t="str">
         <f t="shared" si="10"/>
         <v>x</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:12">
       <c r="B56" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I56" s="2" t="str">
         <f>IF(E56&lt;&gt;"x","x","")</f>
@@ -2824,32 +2701,32 @@
         <v>x</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L56" s="2" t="str">
         <f t="shared" si="10"/>
         <v>x</v>
       </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:12">
       <c r="B57" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I57" s="2" t="str">
         <f>IF(E57&lt;&gt;"x","x","")</f>
@@ -2860,14 +2737,14 @@
         <v>x</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L57" s="2" t="str">
         <f t="shared" si="10"/>
         <v>x</v>
       </c>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:12">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -2880,7 +2757,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:12">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2893,28 +2770,28 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:12">
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:12">
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:12">
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:12">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -2927,7 +2804,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:12">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -2940,7 +2817,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:12">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -2953,7 +2830,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:12">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -2966,168 +2843,168 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:12">
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:12">
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:12">
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:12">
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:12">
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:12">
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:12">
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:12">
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:12">
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:12">
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:12">
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:12">
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:12">
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:12">
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="8:12">
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="8:12">
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="8:12">
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="8:12">
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="8:12">
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="8:12">
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="8:12">
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="8:12">
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="8:12">
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="8:12">
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
@@ -3141,7 +3018,7 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1:L1 Q11:U11 B63:L66 B91:L1048576 H67:L90 B5:G59 H58:L62 B4:I4 J4:L57 H5:I57 O3 B3:L3 B2:C2 E2 H2:L2">
+  <conditionalFormatting sqref="B1:L1 P11:T11 B63:L66 B91:L1048576 H67:L90 B5:G59 H58:L62 B4:I4 J4:L57 H5:I57 B2:C2 E2 H2:L2 B3:N3">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"s"</formula>
     </cfRule>
@@ -3152,7 +3029,7 @@
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:L1048576">
+  <conditionalFormatting sqref="H1:L1048576 M3">
     <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"ok"</formula>
     </cfRule>

</xml_diff>

<commit_message>
update excel row 8 -> 1/2r
</commit_message>
<xml_diff>
--- a/states and actions.xlsx
+++ b/states and actions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rothe/github/arg2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF4B401-F019-D649-BCF6-63EC76C2E1D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D1151E-12CF-4149-8656-DEAB12C3B9EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33020" windowHeight="21080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -709,10 +709,10 @@
   <dimension ref="B1:T90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="181" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="13" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="13" ySplit="3" topLeftCell="N25" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -969,7 +969,7 @@
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
update Excel sheet and code
slightly clearer nomenclature and fancier color codes in the sheet, names of errors matched in the code.
</commit_message>
<xml_diff>
--- a/states and actions.xlsx
+++ b/states and actions.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11111"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rothe/github/arg2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domberg\Desktop\studies\2019 ARG2 simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D1151E-12CF-4149-8656-DEAB12C3B9EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33020" windowHeight="21080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="33024" windowHeight="21084"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$B$1:$L$90</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Domberg, Andreas</author>
   </authors>
   <commentList>
-    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="J4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="H36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="35">
   <si>
     <t>rare</t>
   </si>
@@ -174,9 +173,6 @@
     <t>r</t>
   </si>
   <si>
-    <t>1/2r</t>
-  </si>
-  <si>
     <t>r: minor risk of running out of the long frequent feature</t>
   </si>
   <si>
@@ -199,13 +195,19 @@
   </si>
   <si>
     <t>long</t>
+  </si>
+  <si>
+    <t>r/2</t>
+  </si>
+  <si>
+    <t>RR/2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,9 +345,93 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill patternType="lightVertical">
+          <fgColor theme="0"/>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightVertical">
+          <fgColor theme="0"/>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -425,9 +511,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFFFE1FF"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FFFF99CC"/>
+      <color rgb="FFFFE1FF"/>
       <color rgb="FFCCFFCC"/>
       <color rgb="FFFFCCCC"/>
     </mruColors>
@@ -705,25 +791,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="181" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="13" ySplit="3" topLeftCell="N25" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G36" sqref="G36"/>
+      <selection pane="bottomRight" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="7" width="5.83203125" style="1" customWidth="1"/>
-    <col min="8" max="12" width="5.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="52.5" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="2" max="7" width="5.77734375" style="1" customWidth="1"/>
+    <col min="8" max="12" width="9.21875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="52.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
@@ -743,7 +829,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="2:20">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="8" t="s">
         <v>20</v>
@@ -760,10 +846,10 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="N2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="2:20">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -780,7 +866,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>4</v>
@@ -798,13 +884,13 @@
         <v>8</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="2:20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
@@ -843,7 +929,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:20">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -854,14 +940,14 @@
         <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" s="2" t="str">
         <f>IF(E5&lt;&gt;"x","x","")</f>
@@ -878,10 +964,10 @@
         <v>x</v>
       </c>
       <c r="N5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="2:20">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
@@ -892,14 +978,14 @@
         <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="I6" s="2" t="str">
         <f>IF(E6&lt;&gt;"x","x","")</f>
@@ -916,7 +1002,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="7" spans="2:20">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
@@ -930,11 +1016,11 @@
         <v>13</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>17</v>
@@ -948,10 +1034,10 @@
         <v>x</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="2:20">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -965,11 +1051,11 @@
         <v>13</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>17</v>
@@ -986,7 +1072,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:20">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
@@ -997,14 +1083,14 @@
         <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I9" s="2" t="str">
         <f>IF(E9&lt;&gt;"x","x","")</f>
@@ -1018,10 +1104,10 @@
         <v>17</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1032,14 +1118,14 @@
         <v>19</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" s="2" t="str">
         <f>IF(E10&lt;&gt;"x","x","")</f>
@@ -1056,7 +1142,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:20">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1067,10 +1153,10 @@
         <v>19</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
@@ -1096,7 +1182,7 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="2:20">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1107,10 +1193,10 @@
         <v>19</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
@@ -1131,7 +1217,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:20">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1167,7 +1253,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="14" spans="2:20">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1178,14 +1264,14 @@
         <v>19</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="I14" s="2" t="str">
         <f>IF(E14&lt;&gt;"x","x","")</f>
@@ -1203,7 +1289,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="15" spans="2:20">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1214,14 +1300,14 @@
         <v>19</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="I15" s="2" t="str">
         <f>IF(E15&lt;&gt;"x","x","")</f>
@@ -1239,7 +1325,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="16" spans="2:20">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
@@ -1253,7 +1339,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
@@ -1274,7 +1360,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
@@ -1288,7 +1374,7 @@
         <v>13</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
@@ -1309,7 +1395,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
@@ -1320,10 +1406,10 @@
         <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
@@ -1345,7 +1431,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
@@ -1356,10 +1442,10 @@
         <v>19</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
@@ -1381,7 +1467,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
@@ -1392,10 +1478,10 @@
         <v>19</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
@@ -1417,7 +1503,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
@@ -1428,10 +1514,10 @@
         <v>19</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
@@ -1453,7 +1539,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>12</v>
       </c>
@@ -1489,7 +1575,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>12</v>
       </c>
@@ -1500,14 +1586,14 @@
         <v>14</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I23" s="2" t="str">
         <f>IF(E23&lt;&gt;"x","x","")</f>
@@ -1524,7 +1610,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>12</v>
       </c>
@@ -1535,7 +1621,7 @@
         <v>14</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>13</v>
@@ -1559,7 +1645,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="25" spans="2:12">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>12</v>
       </c>
@@ -1573,11 +1659,11 @@
         <v>13</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>17</v>
@@ -1595,7 +1681,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="26" spans="2:12">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>12</v>
       </c>
@@ -1609,11 +1695,11 @@
         <v>13</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>17</v>
@@ -1631,7 +1717,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="27" spans="2:12">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>12</v>
       </c>
@@ -1642,14 +1728,14 @@
         <v>14</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I27" s="2" t="str">
         <f>IF(E27&lt;&gt;"x","x","")</f>
@@ -1667,7 +1753,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="28" spans="2:12">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>12</v>
       </c>
@@ -1678,14 +1764,14 @@
         <v>14</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I28" s="2" t="str">
         <f>IF(E28&lt;&gt;"x","x","")</f>
@@ -1703,7 +1789,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="29" spans="2:12">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>12</v>
       </c>
@@ -1714,10 +1800,10 @@
         <v>14</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
@@ -1739,7 +1825,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="30" spans="2:12">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>12</v>
       </c>
@@ -1750,10 +1836,10 @@
         <v>14</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
@@ -1775,7 +1861,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="31" spans="2:12">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>15</v>
       </c>
@@ -1811,7 +1897,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="32" spans="2:12">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
         <v>15</v>
       </c>
@@ -1822,7 +1908,7 @@
         <v>19</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>13</v>
@@ -1846,7 +1932,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="33" spans="2:12">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
         <v>15</v>
       </c>
@@ -1857,14 +1943,14 @@
         <v>19</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="I33" s="2" t="str">
         <f>IF(E33&lt;&gt;"x","x","")</f>
@@ -1881,7 +1967,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="34" spans="2:12">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>15</v>
       </c>
@@ -1895,7 +1981,7 @@
         <v>13</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
@@ -1916,7 +2002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="2:12">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
         <v>15</v>
       </c>
@@ -1930,11 +2016,11 @@
         <v>13</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>17</v>
@@ -1951,7 +2037,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="2:12">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
         <v>15</v>
       </c>
@@ -1962,10 +2048,10 @@
         <v>19</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
@@ -1986,7 +2072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="2:12">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
         <v>15</v>
       </c>
@@ -1997,10 +2083,10 @@
         <v>19</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
@@ -2021,7 +2107,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="2:12">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
         <v>15</v>
       </c>
@@ -2032,10 +2118,10 @@
         <v>19</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
@@ -2056,7 +2142,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="2:12">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
         <v>15</v>
       </c>
@@ -2067,10 +2153,10 @@
         <v>19</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
@@ -2091,7 +2177,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="2:12">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>15</v>
       </c>
@@ -2127,7 +2213,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="41" spans="2:12">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
         <v>15</v>
       </c>
@@ -2138,14 +2224,14 @@
         <v>19</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="I41" s="2" t="str">
         <f>IF(E41&lt;&gt;"x","x","")</f>
@@ -2163,7 +2249,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="42" spans="2:12">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
         <v>15</v>
       </c>
@@ -2174,14 +2260,14 @@
         <v>19</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="I42" s="2" t="str">
         <f>IF(E42&lt;&gt;"x","x","")</f>
@@ -2199,7 +2285,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="43" spans="2:12">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
         <v>15</v>
       </c>
@@ -2213,7 +2299,7 @@
         <v>13</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2" t="s">
@@ -2234,7 +2320,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="2:12">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
         <v>15</v>
       </c>
@@ -2248,7 +2334,7 @@
         <v>13</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2" t="s">
@@ -2269,7 +2355,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="2:12">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>15</v>
       </c>
@@ -2280,10 +2366,10 @@
         <v>19</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2" t="s">
@@ -2305,7 +2391,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="2:12">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>15</v>
       </c>
@@ -2316,10 +2402,10 @@
         <v>19</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2" t="s">
@@ -2341,7 +2427,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="2:12">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>15</v>
       </c>
@@ -2352,10 +2438,10 @@
         <v>19</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2" t="s">
@@ -2377,7 +2463,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="2:12">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
         <v>15</v>
       </c>
@@ -2388,10 +2474,10 @@
         <v>19</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2" t="s">
@@ -2413,7 +2499,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="2:12">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
         <v>15</v>
       </c>
@@ -2449,7 +2535,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="50" spans="2:12">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
         <v>15</v>
       </c>
@@ -2460,7 +2546,7 @@
         <v>14</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>13</v>
@@ -2484,7 +2570,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="51" spans="2:12">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
         <v>15</v>
       </c>
@@ -2495,7 +2581,7 @@
         <v>14</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>13</v>
@@ -2519,7 +2605,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="52" spans="2:12">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
         <v>15</v>
       </c>
@@ -2533,7 +2619,7 @@
         <v>13</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2" t="s">
@@ -2555,7 +2641,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="53" spans="2:12">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B53" s="2" t="s">
         <v>15</v>
       </c>
@@ -2569,7 +2655,7 @@
         <v>13</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2" t="s">
@@ -2591,7 +2677,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="54" spans="2:12">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
         <v>15</v>
       </c>
@@ -2602,10 +2688,10 @@
         <v>14</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2" t="s">
@@ -2627,7 +2713,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="55" spans="2:12">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B55" s="2" t="s">
         <v>15</v>
       </c>
@@ -2638,10 +2724,10 @@
         <v>14</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2" t="s">
@@ -2663,7 +2749,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="56" spans="2:12">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B56" s="2" t="s">
         <v>15</v>
       </c>
@@ -2674,10 +2760,10 @@
         <v>14</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2" t="s">
@@ -2699,7 +2785,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="57" spans="2:12">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
         <v>15</v>
       </c>
@@ -2710,10 +2796,10 @@
         <v>14</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2" t="s">
@@ -2735,7 +2821,7 @@
         <v>x</v>
       </c>
     </row>
-    <row r="58" spans="2:12">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -2748,7 +2834,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="2:12">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2761,28 +2847,28 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="2:12">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="2:12">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="2:12">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="2:12">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -2795,7 +2881,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="2:12">
+    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -2808,7 +2894,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="2:12">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -2821,7 +2907,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="2:12">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -2834,168 +2920,168 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="2:12">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="2:12">
+    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="2:12">
+    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="2:12">
+    <row r="70" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="2:12">
+    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="2:12">
+    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="2:12">
+    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="2:12">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="2:12">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="2:12">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="2:12">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="2:12">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="2:12">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="2:12">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="8:12">
+    <row r="81" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="8:12">
+    <row r="82" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="8:12">
+    <row r="83" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="8:12">
+    <row r="84" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="8:12">
+    <row r="85" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="8:12">
+    <row r="86" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="8:12">
+    <row r="87" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="8:12">
+    <row r="88" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="8:12">
+    <row r="89" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="8:12">
+    <row r="90" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
@@ -3010,43 +3096,48 @@
     <mergeCell ref="E2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:L1 P11:T11 B63:L66 B91:L1048576 H67:L90 B5:G59 H58:L62 B4:I4 J4:L57 H5:I57 B2:C2 E2 H2:L2 B3:N3">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"s"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"l"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:L1048576 M3">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"[   ]"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:L1048576">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:L57">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"1/2r"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"r/2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"r"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"RR"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:L1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"RR/2"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rethink states and actions
- In a second pass, reconsidered what we think about risk, relevance and search cost.
- Exclude plots from git.
</commit_message>
<xml_diff>
--- a/states and actions.xlsx
+++ b/states and actions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domberg\Desktop\studies\2019 ARG2 simulations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domberg\Desktop\studies\2019 ARG2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,77 +26,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Domberg, Andreas</author>
-  </authors>
-  <commentList>
-    <comment ref="J4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Domberg, Andreas:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">only really unnecessary if A turns out short
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H36" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Domberg, Andreas:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-2r in fact
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="43">
   <si>
     <t>rare</t>
   </si>
@@ -146,9 +77,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>ok</t>
   </si>
   <si>
@@ -164,18 +92,9 @@
     <t>card</t>
   </si>
   <si>
-    <t>E: query unnecessary information</t>
-  </si>
-  <si>
     <t>1/2e: e when the feature is not known, so could be also short anyway (p=1/2)</t>
   </si>
   <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>r: minor risk of running out of the long frequent feature</t>
-  </si>
-  <si>
     <t>R: risk of loss of rare long feature</t>
   </si>
   <si>
@@ -201,45 +120,55 @@
   </si>
   <si>
     <t>RR/2</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>RR: knowingly waste rare feature</t>
+  </si>
+  <si>
+    <t>RR/2: risk wasting rare feature (it's hidden)</t>
+  </si>
+  <si>
+    <t>P, RR/2</t>
+  </si>
+  <si>
+    <t>P, RR</t>
+  </si>
+  <si>
+    <t>irrel</t>
+  </si>
+  <si>
+    <t>irrel: query unnecessary information</t>
+  </si>
+  <si>
+    <t>irrel, R</t>
+  </si>
+  <si>
+    <t>r-</t>
+  </si>
+  <si>
+    <t>r-: minor risk of running out of the long frequent feature</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>cost: in principle: you waste a known long feature; won't happen much</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -347,15 +276,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill patternType="lightVertical">
-          <fgColor theme="0"/>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <fill>
         <patternFill patternType="lightVertical">
@@ -374,6 +295,14 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightVertical">
+          <fgColor theme="0"/>
           <bgColor rgb="FFFFCCFF"/>
         </patternFill>
       </fill>
@@ -435,6 +364,21 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightVertical">
+          <fgColor theme="0"/>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF99CC"/>
         </patternFill>
       </fill>
@@ -448,15 +392,9 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+        <patternFill patternType="lightVertical">
+          <fgColor theme="0"/>
+          <bgColor rgb="FFFFCCFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -791,14 +729,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B28" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N18" sqref="N18"/>
+      <selection pane="bottomRight" activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,17 +764,17 @@
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="N1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="4"/>
@@ -846,7 +784,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
@@ -866,7 +804,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>4</v>
@@ -884,10 +822,10 @@
         <v>8</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
@@ -895,10 +833,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -912,10 +850,10 @@
         <v>x</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="K4" s="2" t="str">
         <f>IF(OR(C4="full",E4="x"),"x","")</f>
@@ -926,7 +864,7 @@
         <v>x</v>
       </c>
       <c r="N4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
@@ -934,37 +872,37 @@
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I5" s="2" t="str">
         <f>IF(E5&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L5" s="2" t="str">
         <f>IF(OR(D5="full",F5="x"),"x","")</f>
         <v>x</v>
       </c>
       <c r="N5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
@@ -972,34 +910,37 @@
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="I6" s="2" t="str">
         <f>IF(E6&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="L6" s="2" t="str">
         <f>IF(OR(D6="full",F6="x"),"x","")</f>
         <v>x</v>
+      </c>
+      <c r="N6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
@@ -1007,23 +948,23 @@
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J7" s="2" t="str">
         <f t="shared" ref="J7:J12" si="0">IF(F7&lt;&gt;"x","x","")</f>
@@ -1034,7 +975,10 @@
         <v>x</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="N7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
@@ -1042,23 +986,23 @@
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1069,7 +1013,10 @@
         <v>x</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>18</v>
+        <v>34</v>
+      </c>
+      <c r="N8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.3">
@@ -1077,20 +1024,20 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I9" s="2" t="str">
         <f>IF(E9&lt;&gt;"x","x","")</f>
@@ -1101,10 +1048,10 @@
         <v>x</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
@@ -1112,20 +1059,20 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I10" s="2" t="str">
         <f>IF(E10&lt;&gt;"x","x","")</f>
@@ -1136,10 +1083,10 @@
         <v>x</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.3">
@@ -1147,20 +1094,20 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I11" s="2" t="str">
         <f>IF(E11&lt;&gt;"x","x","")</f>
@@ -1171,10 +1118,10 @@
         <v>x</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
@@ -1187,20 +1134,20 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I12" s="2" t="str">
         <f>IF(E12&lt;&gt;"x","x","")</f>
@@ -1211,10 +1158,10 @@
         <v>x</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
@@ -1225,7 +1172,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>13</v>
@@ -1239,10 +1186,10 @@
         <v>x</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K13" s="2" t="str">
         <f t="shared" ref="K13:L15" si="1">IF(OR(C13="full",E13="x"),"x","")</f>
@@ -1261,24 +1208,24 @@
         <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I14" s="2" t="str">
         <f>IF(E14&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K14" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1297,24 +1244,24 @@
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I15" s="2" t="str">
         <f>IF(E15&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K15" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1333,20 +1280,20 @@
         <v>14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="J16" s="2" t="str">
         <f t="shared" ref="J16:J21" si="2">IF(F16&lt;&gt;"x","x","")</f>
@@ -1357,7 +1304,7 @@
         <v>x</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
@@ -1368,20 +1315,20 @@
         <v>14</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="J17" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1392,7 +1339,7 @@
         <v>x</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
@@ -1403,17 +1350,17 @@
         <v>14</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="I18" s="2" t="str">
         <f>IF(E18&lt;&gt;"x","x","")</f>
@@ -1428,7 +1375,7 @@
         <v>x</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
@@ -1439,17 +1386,17 @@
         <v>14</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I19" s="2" t="str">
         <f>IF(E19&lt;&gt;"x","x","")</f>
@@ -1464,7 +1411,7 @@
         <v>x</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
@@ -1475,17 +1422,17 @@
         <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="I20" s="2" t="str">
         <f>IF(E20&lt;&gt;"x","x","")</f>
@@ -1500,7 +1447,7 @@
         <v>x</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
@@ -1511,17 +1458,17 @@
         <v>14</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I21" s="2" t="str">
         <f>IF(E21&lt;&gt;"x","x","")</f>
@@ -1536,7 +1483,7 @@
         <v>x</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
@@ -1544,7 +1491,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>14</v>
@@ -1561,10 +1508,10 @@
         <v>x</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="K22" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1580,30 +1527,30 @@
         <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I23" s="2" t="str">
         <f>IF(E23&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L23" s="2" t="str">
         <f t="shared" si="4"/>
@@ -1615,30 +1562,30 @@
         <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I24" s="2" t="str">
         <f>IF(E24&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L24" s="2" t="str">
         <f t="shared" si="4"/>
@@ -1650,7 +1597,7 @@
         <v>12</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>14</v>
@@ -1659,14 +1606,14 @@
         <v>13</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J25" s="2" t="str">
         <f t="shared" ref="J25:J30" si="5">IF(F25&lt;&gt;"x","x","")</f>
@@ -1686,7 +1633,7 @@
         <v>12</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>14</v>
@@ -1695,14 +1642,14 @@
         <v>13</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J26" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1722,20 +1669,20 @@
         <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I27" s="2" t="str">
         <f>IF(E27&lt;&gt;"x","x","")</f>
@@ -1746,7 +1693,7 @@
         <v>x</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L27" s="2" t="str">
         <f t="shared" si="4"/>
@@ -1758,20 +1705,20 @@
         <v>12</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I28" s="2" t="str">
         <f>IF(E28&lt;&gt;"x","x","")</f>
@@ -1782,7 +1729,7 @@
         <v>x</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L28" s="2" t="str">
         <f t="shared" si="4"/>
@@ -1794,20 +1741,20 @@
         <v>12</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I29" s="2" t="str">
         <f>IF(E29&lt;&gt;"x","x","")</f>
@@ -1818,7 +1765,7 @@
         <v>x</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L29" s="2" t="str">
         <f t="shared" si="4"/>
@@ -1830,20 +1777,20 @@
         <v>12</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I30" s="2" t="str">
         <f>IF(E30&lt;&gt;"x","x","")</f>
@@ -1854,7 +1801,7 @@
         <v>x</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L30" s="2" t="str">
         <f t="shared" si="4"/>
@@ -1866,10 +1813,10 @@
         <v>15</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>13</v>
@@ -1883,10 +1830,10 @@
         <v>x</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K31" s="2" t="str">
         <f>IF(OR(C31="full",E31="x"),"x","")</f>
@@ -1902,30 +1849,30 @@
         <v>15</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I32" s="2" t="str">
         <f>IF(E32&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L32" s="2" t="str">
         <f t="shared" si="4"/>
@@ -1937,30 +1884,30 @@
         <v>15</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="I33" s="2" t="str">
         <f>IF(E33&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="L33" s="2" t="str">
         <f t="shared" si="4"/>
@@ -1972,23 +1919,23 @@
         <v>15</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J34" s="2" t="str">
         <f t="shared" ref="J34:J39" si="6">IF(F34&lt;&gt;"x","x","")</f>
@@ -1999,7 +1946,7 @@
         <v>x</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.3">
@@ -2007,23 +1954,23 @@
         <v>15</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J35" s="2" t="str">
         <f t="shared" si="6"/>
@@ -2034,7 +1981,7 @@
         <v>x</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.3">
@@ -2042,20 +1989,20 @@
         <v>15</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I36" s="2" t="str">
         <f>IF(E36&lt;&gt;"x","x","")</f>
@@ -2066,10 +2013,10 @@
         <v>x</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.3">
@@ -2077,20 +2024,20 @@
         <v>15</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I37" s="2" t="str">
         <f>IF(E37&lt;&gt;"x","x","")</f>
@@ -2101,10 +2048,10 @@
         <v>x</v>
       </c>
       <c r="K37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L37" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.3">
@@ -2112,20 +2059,20 @@
         <v>15</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I38" s="2" t="str">
         <f>IF(E38&lt;&gt;"x","x","")</f>
@@ -2136,10 +2083,10 @@
         <v>x</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.3">
@@ -2147,20 +2094,20 @@
         <v>15</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I39" s="2" t="str">
         <f>IF(E39&lt;&gt;"x","x","")</f>
@@ -2171,10 +2118,10 @@
         <v>x</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.3">
@@ -2185,7 +2132,7 @@
         <v>14</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>13</v>
@@ -2199,10 +2146,10 @@
         <v>x</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K40" s="2" t="str">
         <f t="shared" ref="K40:L42" si="7">IF(OR(C40="full",E40="x"),"x","")</f>
@@ -2221,24 +2168,24 @@
         <v>14</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="I41" s="2" t="str">
         <f>IF(E41&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K41" s="2" t="str">
         <f t="shared" si="7"/>
@@ -2257,24 +2204,24 @@
         <v>14</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="6" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="I42" s="2" t="str">
         <f>IF(E42&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K42" s="2" t="str">
         <f t="shared" si="7"/>
@@ -2293,20 +2240,20 @@
         <v>14</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="J43" s="2" t="str">
         <f t="shared" ref="J43:J48" si="8">IF(F43&lt;&gt;"x","x","")</f>
@@ -2317,7 +2264,7 @@
         <v>x</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.3">
@@ -2328,20 +2275,20 @@
         <v>14</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="J44" s="2" t="str">
         <f t="shared" si="8"/>
@@ -2352,7 +2299,7 @@
         <v>x</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.3">
@@ -2363,17 +2310,17 @@
         <v>14</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I45" s="2" t="str">
         <f>IF(E45&lt;&gt;"x","x","")</f>
@@ -2388,7 +2335,7 @@
         <v>x</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.3">
@@ -2399,17 +2346,17 @@
         <v>14</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I46" s="2" t="str">
         <f>IF(E46&lt;&gt;"x","x","")</f>
@@ -2424,7 +2371,7 @@
         <v>x</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.3">
@@ -2435,17 +2382,17 @@
         <v>14</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I47" s="2" t="str">
         <f>IF(E47&lt;&gt;"x","x","")</f>
@@ -2460,7 +2407,7 @@
         <v>x</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.3">
@@ -2471,17 +2418,17 @@
         <v>14</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I48" s="2" t="str">
         <f>IF(E48&lt;&gt;"x","x","")</f>
@@ -2496,7 +2443,7 @@
         <v>x</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.3">
@@ -2504,7 +2451,7 @@
         <v>15</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>14</v>
@@ -2521,10 +2468,10 @@
         <v>x</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="K49" s="2" t="str">
         <f t="shared" si="9"/>
@@ -2540,30 +2487,30 @@
         <v>15</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I50" s="2" t="str">
         <f>IF(E50&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L50" s="2" t="str">
         <f t="shared" si="10"/>
@@ -2575,30 +2522,30 @@
         <v>15</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I51" s="2" t="str">
         <f>IF(E51&lt;&gt;"x","x","")</f>
         <v>x</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L51" s="2" t="str">
         <f t="shared" si="10"/>
@@ -2610,7 +2557,7 @@
         <v>15</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>14</v>
@@ -2619,14 +2566,14 @@
         <v>13</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J52" s="2" t="str">
         <f t="shared" ref="J52:J57" si="11">IF(F52&lt;&gt;"x","x","")</f>
@@ -2646,7 +2593,7 @@
         <v>15</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>14</v>
@@ -2655,14 +2602,14 @@
         <v>13</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J53" s="2" t="str">
         <f t="shared" si="11"/>
@@ -2682,20 +2629,20 @@
         <v>15</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I54" s="2" t="str">
         <f>IF(E54&lt;&gt;"x","x","")</f>
@@ -2706,7 +2653,7 @@
         <v>x</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L54" s="2" t="str">
         <f t="shared" si="10"/>
@@ -2718,20 +2665,20 @@
         <v>15</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I55" s="2" t="str">
         <f>IF(E55&lt;&gt;"x","x","")</f>
@@ -2742,7 +2689,7 @@
         <v>x</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L55" s="2" t="str">
         <f t="shared" si="10"/>
@@ -2754,20 +2701,20 @@
         <v>15</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I56" s="2" t="str">
         <f>IF(E56&lt;&gt;"x","x","")</f>
@@ -2778,7 +2725,7 @@
         <v>x</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L56" s="2" t="str">
         <f t="shared" si="10"/>
@@ -2790,20 +2737,20 @@
         <v>15</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I57" s="2" t="str">
         <f>IF(E57&lt;&gt;"x","x","")</f>
@@ -2814,7 +2761,7 @@
         <v>x</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L57" s="2" t="str">
         <f t="shared" si="10"/>
@@ -3096,52 +3043,51 @@
     <mergeCell ref="E2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:L1 P11:T11 B63:L66 B91:L1048576 H67:L90 B5:G59 H58:L62 B4:I4 J4:L57 H5:I57 B2:C2 E2 H2:L2 B3:N3">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
       <formula>"s"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
       <formula>"l"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:L1048576 M3">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>"[   ]"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:L1048576">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:L57">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
-      <formula>"E"</formula>
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+      <formula>"irrel"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"r/2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"r"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"RR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:L1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"RR/2"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>